<commit_message>
completed more formatting of plots
</commit_message>
<xml_diff>
--- a/00_data/Descriptives for 3 variables.xlsx
+++ b/00_data/Descriptives for 3 variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\BIDAMIA_GoogleDrive\BIDAMIA_Projects\Upwork\mental_health_covid\00_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4419E6F3-354D-4AB2-8282-0F3DAFCA34A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18E2A2E-EC06-466C-9D87-819D39497C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{F57DC66E-35EB-4BF0-98F4-6A0539E03339}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -559,13 +559,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>0.15690000000000001</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="D8">
-        <v>0.2114</v>
+        <v>0.1085</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
@@ -573,13 +573,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>0.154</v>
+        <v>0.15690000000000001</v>
       </c>
       <c r="D9">
-        <v>0.1605</v>
+        <v>0.2114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
@@ -587,13 +587,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>0.1358</v>
+        <v>0.154</v>
       </c>
       <c r="D10">
-        <v>9.2200000000000004E-2</v>
+        <v>0.1605</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
@@ -601,13 +601,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>0.23799999999999999</v>
+        <v>0.1358</v>
       </c>
       <c r="D11">
-        <v>0.1085</v>
+        <v>9.2200000000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">

</xml_diff>